<commit_message>
Ready for the hardware
</commit_message>
<xml_diff>
--- a/schema/airsens_v3_0_impantation.xlsx
+++ b/schema/airsens_v3_0_impantation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f34ccaa6039d8a87/technique/_projets/esp32-micropython/esp32-airsens-v3/schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C32B5C8-5F9F-434E-B70B-921D89E37F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="8_{4C32B5C8-5F9F-434E-B70B-921D89E37F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7135DFA-AF6E-482F-A0B4-0F1CC775DC45}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1065" windowWidth="23490" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="airsens v1.0 proto" sheetId="9" r:id="rId1"/>
     <sheet name="airsens v1.1 proto" sheetId="10" r:id="rId2"/>
+    <sheet name="airsens v3.0 proto" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'airsens v1.0 proto'!$A$1:$Q$24</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="54">
   <si>
     <t>GND</t>
   </si>
@@ -182,12 +183,41 @@
   <si>
     <t>Sensor</t>
   </si>
+  <si>
+    <t>SW-PAIR</t>
+  </si>
+  <si>
+    <t>IO14</t>
+  </si>
+  <si>
+    <t>LED-K</t>
+  </si>
+  <si>
+    <t>LED-A</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>PAIR
+IO14</t>
+  </si>
+  <si>
+    <t>LED
+IO12</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32</t>
+  </si>
+  <si>
+    <t>I2C - sensor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +255,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -431,8 +468,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="46">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1001,11 +1050,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1377,25 +1483,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1413,9 +1567,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1428,50 +1579,29 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1524,29 +1654,238 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1556,6 +1895,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFF33"/>
+      <color rgb="FF99FF66"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFCC6600"/>
       <color rgb="FFFFCCFF"/>
@@ -1564,8 +1905,6 @@
       <color rgb="FF66FFFF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FFCCCCFF"/>
-      <color rgb="FFCCFFCC"/>
-      <color rgb="FFCCFFFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1961,6 +2300,139 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>264582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>709083</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Ellipse 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1227E1B4-16D5-450E-983E-96A3E0169A6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3111499" y="1428749"/>
+          <a:ext cx="698501" cy="666751"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>264582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>709083</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Ellipse 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC1C036-8C7E-417D-B470-E65FAB0F7718}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3103114" y="1427374"/>
+          <a:ext cx="698501" cy="654107"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2229,7 +2701,7 @@
   </sheetPr>
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
@@ -2245,36 +2717,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="K1" s="131" t="s">
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="K1" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="131"/>
-      <c r="M1" s="131"/>
-      <c r="N1" s="131"/>
-      <c r="O1" s="131"/>
-      <c r="P1" s="131"/>
-      <c r="Q1" s="131"/>
+      <c r="L1" s="132"/>
+      <c r="M1" s="132"/>
+      <c r="N1" s="132"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="137" t="s">
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="137"/>
+      <c r="F2" s="140"/>
       <c r="G2" s="4">
         <v>6</v>
       </c>
@@ -2289,15 +2761,15 @@
       <c r="L2" s="4">
         <v>6</v>
       </c>
-      <c r="M2" s="137" t="s">
+      <c r="M2" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="137"/>
-      <c r="O2" s="137" t="s">
+      <c r="N2" s="140"/>
+      <c r="O2" s="140" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="140"/>
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2402,14 +2874,14 @@
       <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="148" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="138"/>
-      <c r="E6" s="139"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="154"/>
       <c r="F6" s="24" t="s">
         <v>1</v>
       </c>
@@ -2430,12 +2902,12 @@
       <c r="M6" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="N6" s="144"/>
-      <c r="O6" s="154"/>
-      <c r="P6" s="127" t="s">
+      <c r="N6" s="127"/>
+      <c r="O6" s="141"/>
+      <c r="P6" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="Q6" s="149" t="s">
+      <c r="Q6" s="135" t="s">
         <v>0</v>
       </c>
       <c r="R6" s="16">
@@ -2446,10 +2918,10 @@
       <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="133"/>
-      <c r="C7" s="135"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="141"/>
+      <c r="B7" s="149"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="156"/>
       <c r="G7" s="17" t="s">
         <v>15</v>
       </c>
@@ -2464,10 +2936,10 @@
       <c r="L7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="155"/>
-      <c r="O7" s="156"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="150"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="134"/>
+      <c r="Q7" s="136"/>
       <c r="R7" s="16">
         <v>5</v>
       </c>
@@ -2520,13 +2992,13 @@
       <c r="A10" s="14">
         <v>8</v>
       </c>
-      <c r="B10" s="125" t="s">
+      <c r="B10" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="127" t="s">
+      <c r="C10" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="129" t="s">
+      <c r="D10" s="146" t="s">
         <v>2</v>
       </c>
       <c r="F10" s="27" t="s">
@@ -2553,13 +3025,13 @@
       <c r="M10" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="O10" s="151" t="s">
+      <c r="O10" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="127" t="s">
+      <c r="P10" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" s="149" t="s">
+      <c r="Q10" s="135" t="s">
         <v>0</v>
       </c>
       <c r="R10" s="16">
@@ -2570,9 +3042,9 @@
       <c r="A11" s="14">
         <v>9</v>
       </c>
-      <c r="B11" s="126"/>
-      <c r="C11" s="128"/>
-      <c r="D11" s="130"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="134"/>
+      <c r="D11" s="147"/>
       <c r="F11" s="28" t="s">
         <v>19</v>
       </c>
@@ -2597,9 +3069,9 @@
       <c r="M11" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="152"/>
-      <c r="P11" s="128"/>
-      <c r="Q11" s="153"/>
+      <c r="O11" s="138"/>
+      <c r="P11" s="134"/>
+      <c r="Q11" s="139"/>
       <c r="R11" s="16">
         <v>9</v>
       </c>
@@ -2723,13 +3195,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="60"/>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="36"/>
       <c r="I16" s="16">
         <v>14</v>
@@ -2738,13 +3210,13 @@
         <v>14</v>
       </c>
       <c r="K16" s="38"/>
-      <c r="L16" s="142" t="s">
+      <c r="L16" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="142"/>
-      <c r="N16" s="142"/>
-      <c r="O16" s="142"/>
-      <c r="P16" s="142"/>
+      <c r="M16" s="125"/>
+      <c r="N16" s="125"/>
+      <c r="O16" s="125"/>
+      <c r="P16" s="125"/>
       <c r="Q16" s="59"/>
       <c r="R16" s="16">
         <v>14</v>
@@ -2757,11 +3229,11 @@
       <c r="B17" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="125"/>
       <c r="H17" s="59"/>
       <c r="I17" s="16">
         <v>15</v>
@@ -2770,11 +3242,11 @@
         <v>15</v>
       </c>
       <c r="K17" s="60"/>
-      <c r="L17" s="142"/>
-      <c r="M17" s="142"/>
-      <c r="N17" s="142"/>
-      <c r="O17" s="142"/>
-      <c r="P17" s="142"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="125"/>
+      <c r="N17" s="125"/>
+      <c r="O17" s="125"/>
+      <c r="P17" s="125"/>
       <c r="Q17" s="42" t="s">
         <v>26</v>
       </c>
@@ -2789,11 +3261,11 @@
       <c r="B18" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="142"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="142"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="125"/>
       <c r="H18" s="51" t="s">
         <v>23</v>
       </c>
@@ -2806,11 +3278,11 @@
       <c r="K18" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="142"/>
-      <c r="M18" s="142"/>
-      <c r="N18" s="142"/>
-      <c r="O18" s="142"/>
-      <c r="P18" s="142"/>
+      <c r="L18" s="125"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
+      <c r="O18" s="125"/>
+      <c r="P18" s="125"/>
       <c r="Q18" s="53" t="s">
         <v>25</v>
       </c>
@@ -2825,11 +3297,11 @@
       <c r="B19" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="142"/>
-      <c r="D19" s="142"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="142"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="36"/>
       <c r="I19" s="16">
         <v>17</v>
@@ -2838,11 +3310,11 @@
         <v>17</v>
       </c>
       <c r="K19" s="38"/>
-      <c r="L19" s="142"/>
-      <c r="M19" s="142"/>
-      <c r="N19" s="142"/>
-      <c r="O19" s="142"/>
-      <c r="P19" s="142"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="125"/>
+      <c r="O19" s="125"/>
+      <c r="P19" s="125"/>
       <c r="Q19" s="40" t="s">
         <v>11</v>
       </c>
@@ -2857,11 +3329,11 @@
       <c r="B20" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="142"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
       <c r="H20" s="47" t="s">
         <v>22</v>
       </c>
@@ -2874,11 +3346,11 @@
       <c r="K20" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="142"/>
-      <c r="M20" s="142"/>
-      <c r="N20" s="142"/>
-      <c r="O20" s="142"/>
-      <c r="P20" s="142"/>
+      <c r="L20" s="125"/>
+      <c r="M20" s="125"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="125"/>
       <c r="Q20" s="39" t="s">
         <v>10</v>
       </c>
@@ -2893,11 +3365,11 @@
       <c r="B21" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="142"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
       <c r="H21" s="46" t="s">
         <v>21</v>
       </c>
@@ -2910,11 +3382,11 @@
       <c r="K21" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="142"/>
-      <c r="M21" s="142"/>
-      <c r="N21" s="142"/>
-      <c r="O21" s="142"/>
-      <c r="P21" s="142"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="125"/>
       <c r="Q21" s="52" t="s">
         <v>24</v>
       </c>
@@ -2955,32 +3427,32 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="143" t="s">
+      <c r="C23" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="144"/>
-      <c r="E23" s="144"/>
-      <c r="F23" s="144"/>
-      <c r="G23" s="145"/>
-      <c r="L23" s="143" t="s">
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="128"/>
+      <c r="L23" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="M23" s="144"/>
-      <c r="N23" s="144"/>
-      <c r="O23" s="144"/>
-      <c r="P23" s="145"/>
+      <c r="M23" s="127"/>
+      <c r="N23" s="127"/>
+      <c r="O23" s="127"/>
+      <c r="P23" s="128"/>
     </row>
     <row r="24" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="146"/>
-      <c r="D24" s="147"/>
-      <c r="E24" s="147"/>
-      <c r="F24" s="147"/>
-      <c r="G24" s="148"/>
-      <c r="L24" s="146"/>
-      <c r="M24" s="147"/>
-      <c r="N24" s="147"/>
-      <c r="O24" s="147"/>
-      <c r="P24" s="148"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="131"/>
+      <c r="L24" s="129"/>
+      <c r="M24" s="130"/>
+      <c r="N24" s="130"/>
+      <c r="O24" s="130"/>
+      <c r="P24" s="131"/>
     </row>
     <row r="25" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2991,6 +3463,15 @@
     <row r="31" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="D6:E7"/>
     <mergeCell ref="L16:P21"/>
     <mergeCell ref="L23:P24"/>
     <mergeCell ref="C16:G21"/>
@@ -3004,15 +3485,6 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="N6:O7"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="D6:E7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3035,7 +3507,7 @@
   </sheetPr>
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
@@ -3051,36 +3523,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="167"/>
-      <c r="K1" s="165" t="s">
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="175"/>
+      <c r="K1" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="167"/>
+      <c r="L1" s="174"/>
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="174"/>
+      <c r="Q1" s="175"/>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="140" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="137" t="s">
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="137"/>
+      <c r="F2" s="140"/>
       <c r="G2" s="4">
         <v>6</v>
       </c>
@@ -3095,15 +3567,15 @@
       <c r="L2" s="4">
         <v>6</v>
       </c>
-      <c r="M2" s="137" t="s">
+      <c r="M2" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="137"/>
-      <c r="O2" s="137" t="s">
+      <c r="N2" s="140"/>
+      <c r="O2" s="140" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="140"/>
       <c r="R2" s="6"/>
     </row>
     <row r="3" spans="1:18" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3291,10 +3763,10 @@
       <c r="C7" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="157" t="s">
+      <c r="D7" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="158"/>
+      <c r="E7" s="166"/>
       <c r="H7" s="116" t="s">
         <v>41</v>
       </c>
@@ -3305,10 +3777,10 @@
         <v>5</v>
       </c>
       <c r="K7" s="2"/>
-      <c r="N7" s="172" t="s">
+      <c r="N7" s="180" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="173"/>
+      <c r="O7" s="181"/>
       <c r="P7" s="69" t="s">
         <v>5</v>
       </c>
@@ -3329,14 +3801,14 @@
       <c r="C8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="168" t="s">
+      <c r="E8" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="127" t="s">
+      <c r="F8" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="127"/>
-      <c r="H8" s="170" t="s">
+      <c r="G8" s="133"/>
+      <c r="H8" s="178" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="16">
@@ -3345,14 +3817,14 @@
       <c r="J8" s="14">
         <v>6</v>
       </c>
-      <c r="K8" s="176" t="s">
+      <c r="K8" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="127" t="s">
+      <c r="L8" s="133" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="127"/>
-      <c r="N8" s="178" t="s">
+      <c r="M8" s="133"/>
+      <c r="N8" s="161" t="s">
         <v>0</v>
       </c>
       <c r="P8" s="79" t="s">
@@ -3375,20 +3847,20 @@
       <c r="C9" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="169"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
-      <c r="H9" s="171"/>
+      <c r="E9" s="177"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="179"/>
       <c r="I9" s="16">
         <v>7</v>
       </c>
       <c r="J9" s="14">
         <v>7</v>
       </c>
-      <c r="K9" s="177"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-      <c r="N9" s="179"/>
+      <c r="K9" s="160"/>
+      <c r="L9" s="134"/>
+      <c r="M9" s="134"/>
+      <c r="N9" s="162"/>
       <c r="P9" s="94" t="s">
         <v>18</v>
       </c>
@@ -3434,14 +3906,14 @@
       <c r="B11" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="168" t="s">
+      <c r="E11" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="127" t="s">
+      <c r="F11" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="127"/>
-      <c r="H11" s="174" t="s">
+      <c r="G11" s="133"/>
+      <c r="H11" s="157" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="16">
@@ -3450,14 +3922,14 @@
       <c r="J11" s="14">
         <v>9</v>
       </c>
-      <c r="K11" s="180" t="s">
+      <c r="K11" s="163" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="127" t="s">
+      <c r="L11" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="M11" s="127"/>
-      <c r="N11" s="178" t="s">
+      <c r="M11" s="133"/>
+      <c r="N11" s="161" t="s">
         <v>0</v>
       </c>
       <c r="Q11" s="75" t="s">
@@ -3474,20 +3946,20 @@
       <c r="B12" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="169"/>
-      <c r="F12" s="128"/>
-      <c r="G12" s="128"/>
-      <c r="H12" s="175"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="158"/>
       <c r="I12" s="16">
         <v>10</v>
       </c>
       <c r="J12" s="14">
         <v>10</v>
       </c>
-      <c r="K12" s="181"/>
-      <c r="L12" s="128"/>
-      <c r="M12" s="128"/>
-      <c r="N12" s="179"/>
+      <c r="K12" s="164"/>
+      <c r="L12" s="134"/>
+      <c r="M12" s="134"/>
+      <c r="N12" s="162"/>
       <c r="Q12" s="93" t="s">
         <v>8</v>
       </c>
@@ -3574,13 +4046,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="60"/>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
+      <c r="G16" s="125"/>
       <c r="H16" s="36"/>
       <c r="I16" s="16">
         <v>14</v>
@@ -3589,11 +4061,11 @@
         <v>14</v>
       </c>
       <c r="K16" s="38"/>
-      <c r="L16" s="142"/>
-      <c r="M16" s="142"/>
-      <c r="N16" s="142"/>
-      <c r="O16" s="142"/>
-      <c r="P16" s="142"/>
+      <c r="L16" s="125"/>
+      <c r="M16" s="125"/>
+      <c r="N16" s="125"/>
+      <c r="O16" s="125"/>
+      <c r="P16" s="125"/>
       <c r="Q16" s="59"/>
       <c r="R16" s="16">
         <v>14</v>
@@ -3606,11 +4078,11 @@
       <c r="B17" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="125"/>
+      <c r="G17" s="125"/>
       <c r="H17" s="59"/>
       <c r="I17" s="16">
         <v>15</v>
@@ -3619,11 +4091,11 @@
         <v>15</v>
       </c>
       <c r="K17" s="60"/>
-      <c r="L17" s="142"/>
-      <c r="M17" s="142"/>
-      <c r="N17" s="142"/>
-      <c r="O17" s="142"/>
-      <c r="P17" s="142"/>
+      <c r="L17" s="125"/>
+      <c r="M17" s="125"/>
+      <c r="N17" s="125"/>
+      <c r="O17" s="125"/>
+      <c r="P17" s="125"/>
       <c r="Q17" s="82" t="s">
         <v>26</v>
       </c>
@@ -3638,11 +4110,11 @@
       <c r="B18" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="142"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="142"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="142"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
+      <c r="G18" s="125"/>
       <c r="H18" s="76" t="s">
         <v>23</v>
       </c>
@@ -3655,11 +4127,11 @@
       <c r="K18" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="142"/>
-      <c r="M18" s="142"/>
-      <c r="N18" s="142"/>
-      <c r="O18" s="142"/>
-      <c r="P18" s="142"/>
+      <c r="L18" s="125"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
+      <c r="O18" s="125"/>
+      <c r="P18" s="125"/>
       <c r="Q18" s="84" t="s">
         <v>25</v>
       </c>
@@ -3674,11 +4146,11 @@
       <c r="B19" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="142"/>
-      <c r="D19" s="142"/>
-      <c r="E19" s="142"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="142"/>
+      <c r="C19" s="125"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="36"/>
       <c r="I19" s="16">
         <v>17</v>
@@ -3687,11 +4159,11 @@
         <v>17</v>
       </c>
       <c r="K19" s="38"/>
-      <c r="L19" s="142"/>
-      <c r="M19" s="142"/>
-      <c r="N19" s="142"/>
-      <c r="O19" s="142"/>
-      <c r="P19" s="142"/>
+      <c r="L19" s="125"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="125"/>
+      <c r="O19" s="125"/>
+      <c r="P19" s="125"/>
       <c r="Q19" s="40" t="s">
         <v>11</v>
       </c>
@@ -3706,11 +4178,11 @@
       <c r="B20" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="142"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="142"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
       <c r="H20" s="72" t="s">
         <v>22</v>
       </c>
@@ -3723,11 +4195,11 @@
       <c r="K20" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="142"/>
-      <c r="M20" s="142"/>
-      <c r="N20" s="142"/>
-      <c r="O20" s="142"/>
-      <c r="P20" s="142"/>
+      <c r="L20" s="125"/>
+      <c r="M20" s="125"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="125"/>
       <c r="Q20" s="86" t="s">
         <v>10</v>
       </c>
@@ -3742,11 +4214,11 @@
       <c r="B21" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="142"/>
-      <c r="D21" s="142"/>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="142"/>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
       <c r="H21" s="70" t="s">
         <v>21</v>
       </c>
@@ -3759,11 +4231,11 @@
       <c r="K21" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="142"/>
-      <c r="M21" s="142"/>
-      <c r="N21" s="142"/>
-      <c r="O21" s="142"/>
-      <c r="P21" s="142"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="125"/>
       <c r="Q21" s="59" t="s">
         <v>24</v>
       </c>
@@ -3804,32 +4276,32 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="159" t="s">
+      <c r="C23" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="160"/>
-      <c r="E23" s="160"/>
-      <c r="F23" s="160"/>
-      <c r="G23" s="161"/>
-      <c r="L23" s="159" t="s">
+      <c r="D23" s="168"/>
+      <c r="E23" s="168"/>
+      <c r="F23" s="168"/>
+      <c r="G23" s="169"/>
+      <c r="L23" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="M23" s="160"/>
-      <c r="N23" s="160"/>
-      <c r="O23" s="160"/>
-      <c r="P23" s="161"/>
+      <c r="M23" s="168"/>
+      <c r="N23" s="168"/>
+      <c r="O23" s="168"/>
+      <c r="P23" s="169"/>
     </row>
     <row r="24" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="162"/>
-      <c r="D24" s="163"/>
-      <c r="E24" s="163"/>
-      <c r="F24" s="163"/>
-      <c r="G24" s="164"/>
-      <c r="L24" s="162"/>
-      <c r="M24" s="163"/>
-      <c r="N24" s="163"/>
-      <c r="O24" s="163"/>
-      <c r="P24" s="164"/>
+      <c r="C24" s="170"/>
+      <c r="D24" s="171"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="172"/>
+      <c r="L24" s="170"/>
+      <c r="M24" s="171"/>
+      <c r="N24" s="171"/>
+      <c r="O24" s="171"/>
+      <c r="P24" s="172"/>
     </row>
     <row r="25" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3840,15 +4312,6 @@
     <row r="31" spans="1:18" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="D7:E7"/>
     <mergeCell ref="C23:G24"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="C16:G21"/>
@@ -3864,6 +4327,15 @@
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="N7:O7"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3877,4 +4349,987 @@
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD026F7-D06F-4E35-85EE-DF8AF2911234}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="10.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="173" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="175"/>
+      <c r="J1" s="173" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="174"/>
+      <c r="L1" s="174"/>
+      <c r="M1" s="174"/>
+      <c r="N1" s="174"/>
+      <c r="O1" s="174"/>
+      <c r="P1" s="175"/>
+    </row>
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="241">
+        <v>1</v>
+      </c>
+      <c r="C2" s="241">
+        <v>2</v>
+      </c>
+      <c r="D2" s="241">
+        <v>3</v>
+      </c>
+      <c r="E2" s="241">
+        <v>4</v>
+      </c>
+      <c r="F2" s="241">
+        <v>5</v>
+      </c>
+      <c r="G2" s="242">
+        <v>6</v>
+      </c>
+      <c r="H2" s="242">
+        <v>7</v>
+      </c>
+      <c r="I2" s="242"/>
+      <c r="J2" s="241">
+        <v>7</v>
+      </c>
+      <c r="K2" s="241">
+        <v>6</v>
+      </c>
+      <c r="L2" s="241">
+        <v>5</v>
+      </c>
+      <c r="M2" s="241">
+        <v>4</v>
+      </c>
+      <c r="N2" s="241">
+        <v>3</v>
+      </c>
+      <c r="O2" s="241">
+        <v>2</v>
+      </c>
+      <c r="P2" s="241">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="15"/>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="256" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="257"/>
+      <c r="D3" s="258"/>
+      <c r="E3" s="256" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="259"/>
+      <c r="G3" s="256" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="259"/>
+      <c r="J3" s="256" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="259"/>
+      <c r="L3" s="256" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="259"/>
+      <c r="N3" s="256" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="260"/>
+      <c r="P3" s="259"/>
+      <c r="Q3" s="15"/>
+    </row>
+    <row r="4" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="244">
+        <v>1</v>
+      </c>
+      <c r="B4" s="211" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="212" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="213" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="214" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="215" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="216" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="213" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="243">
+        <v>1</v>
+      </c>
+      <c r="J4" s="219" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="220" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="223" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="207" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="208" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="206" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="224" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="244">
+        <v>2</v>
+      </c>
+      <c r="B5" s="190"/>
+      <c r="C5" s="191"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="217" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="218" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="243">
+        <v>2</v>
+      </c>
+      <c r="J5" s="221" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="222" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="194"/>
+      <c r="M5" s="194"/>
+      <c r="N5" s="194"/>
+      <c r="O5" s="194"/>
+      <c r="P5" s="245"/>
+      <c r="Q5" s="244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="244">
+        <v>3</v>
+      </c>
+      <c r="B6" s="113"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="243">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="189"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="188"/>
+      <c r="P6" s="246"/>
+      <c r="Q6" s="244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="244">
+        <v>4</v>
+      </c>
+      <c r="B7" s="192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="150" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="150"/>
+      <c r="E7" s="198" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="189"/>
+      <c r="G7" s="189"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="243">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="189"/>
+      <c r="L7" s="189"/>
+      <c r="M7" s="184" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="150" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="150"/>
+      <c r="P7" s="182" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="244">
+        <v>5</v>
+      </c>
+      <c r="B8" s="193"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="199"/>
+      <c r="F8" s="204" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="197" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="243">
+        <v>5</v>
+      </c>
+      <c r="J8" s="225" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="235" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="185"/>
+      <c r="N8" s="151"/>
+      <c r="O8" s="151"/>
+      <c r="P8" s="183"/>
+      <c r="Q8" s="244">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="244">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="189"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="243">
+        <v>6</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="189"/>
+      <c r="L9" s="189"/>
+      <c r="M9" s="189"/>
+      <c r="N9" s="189"/>
+      <c r="O9" s="189"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="244">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="244">
+        <v>7</v>
+      </c>
+      <c r="B10" s="192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="150" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="150"/>
+      <c r="E10" s="200" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="189"/>
+      <c r="G10" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="115" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="243">
+        <v>7</v>
+      </c>
+      <c r="J10" s="226" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="227" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" s="189"/>
+      <c r="M10" s="186" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="150" t="s">
+        <v>39</v>
+      </c>
+      <c r="O10" s="150"/>
+      <c r="P10" s="182" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="244">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="244">
+        <v>8</v>
+      </c>
+      <c r="B11" s="193"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="151"/>
+      <c r="E11" s="201"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="232" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="234" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="243">
+        <v>8</v>
+      </c>
+      <c r="J11" s="234" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="232" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="189"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="151"/>
+      <c r="O11" s="151"/>
+      <c r="P11" s="183"/>
+      <c r="Q11" s="244">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="244">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="189"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="233" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="233" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="243">
+        <v>9</v>
+      </c>
+      <c r="J12" s="233" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="233" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="189"/>
+      <c r="M12" s="189"/>
+      <c r="N12" s="189"/>
+      <c r="O12" s="189"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="244">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="244">
+        <v>10</v>
+      </c>
+      <c r="B13" s="192" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="150" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="150"/>
+      <c r="E13" s="202" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="189"/>
+      <c r="G13" s="228" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="228" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="243">
+        <v>10</v>
+      </c>
+      <c r="J13" s="228" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="228" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="189"/>
+      <c r="M13" s="236" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="150" t="s">
+        <v>45</v>
+      </c>
+      <c r="O13" s="150"/>
+      <c r="P13" s="182" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="244">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="244">
+        <v>11</v>
+      </c>
+      <c r="B14" s="193"/>
+      <c r="C14" s="151"/>
+      <c r="D14" s="151"/>
+      <c r="E14" s="203"/>
+      <c r="F14" s="189"/>
+      <c r="G14" s="229" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="229" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="243">
+        <v>11</v>
+      </c>
+      <c r="J14" s="229" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="229" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="189"/>
+      <c r="M14" s="237"/>
+      <c r="N14" s="151"/>
+      <c r="O14" s="151"/>
+      <c r="P14" s="183"/>
+      <c r="Q14" s="244">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="244">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="189"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="189"/>
+      <c r="G15" s="189"/>
+      <c r="H15" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="243">
+        <v>12</v>
+      </c>
+      <c r="J15" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="189"/>
+      <c r="L15" s="189"/>
+      <c r="M15" s="189"/>
+      <c r="N15" s="189"/>
+      <c r="O15" s="189"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="244">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="244">
+        <v>13</v>
+      </c>
+      <c r="B16" s="210" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="196" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="195" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="197"/>
+      <c r="F16" s="189"/>
+      <c r="G16" s="189"/>
+      <c r="H16" s="231" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="243">
+        <v>13</v>
+      </c>
+      <c r="J16" s="231" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" s="189"/>
+      <c r="L16" s="189"/>
+      <c r="M16" s="225"/>
+      <c r="N16" s="196" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" s="195" t="s">
+        <v>47</v>
+      </c>
+      <c r="P16" s="238" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" s="244">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="244">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="189"/>
+      <c r="D17" s="189"/>
+      <c r="E17" s="189"/>
+      <c r="F17" s="189"/>
+      <c r="G17" s="189"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="243">
+        <v>14</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="189"/>
+      <c r="L17" s="189"/>
+      <c r="M17" s="189"/>
+      <c r="N17" s="189"/>
+      <c r="O17" s="189"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="244">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="244">
+        <v>15</v>
+      </c>
+      <c r="B18" s="62"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="243">
+        <v>15</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="244">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="244">
+        <v>16</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="125" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="125"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="125"/>
+      <c r="G19" s="125"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="243">
+        <v>16</v>
+      </c>
+      <c r="J19" s="38"/>
+      <c r="K19" s="125" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="125"/>
+      <c r="M19" s="125"/>
+      <c r="N19" s="125"/>
+      <c r="O19" s="125"/>
+      <c r="P19" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" s="244">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="244">
+        <v>17</v>
+      </c>
+      <c r="B20" s="247" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="243">
+        <v>17</v>
+      </c>
+      <c r="J20" s="60"/>
+      <c r="K20" s="125"/>
+      <c r="L20" s="125"/>
+      <c r="M20" s="125"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="252" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q20" s="244">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="244">
+        <v>18</v>
+      </c>
+      <c r="B21" s="248" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="125"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="125"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="243">
+        <v>18</v>
+      </c>
+      <c r="J21" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="253" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q21" s="244">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="244">
+        <v>19</v>
+      </c>
+      <c r="B22" s="249" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="125"/>
+      <c r="D22" s="125"/>
+      <c r="E22" s="125"/>
+      <c r="F22" s="125"/>
+      <c r="G22" s="125"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="243">
+        <v>19</v>
+      </c>
+      <c r="J22" s="38"/>
+      <c r="K22" s="125"/>
+      <c r="L22" s="125"/>
+      <c r="M22" s="125"/>
+      <c r="N22" s="125"/>
+      <c r="O22" s="125"/>
+      <c r="P22" s="254" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="244">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="244">
+        <v>20</v>
+      </c>
+      <c r="B23" s="250" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="125"/>
+      <c r="D23" s="125"/>
+      <c r="E23" s="125"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="243">
+        <v>20</v>
+      </c>
+      <c r="J23" s="85" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="125"/>
+      <c r="L23" s="125"/>
+      <c r="M23" s="125"/>
+      <c r="N23" s="125"/>
+      <c r="O23" s="125"/>
+      <c r="P23" s="255" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" s="244">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="244">
+        <v>21</v>
+      </c>
+      <c r="B24" s="251" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="125"/>
+      <c r="D24" s="125"/>
+      <c r="E24" s="125"/>
+      <c r="F24" s="125"/>
+      <c r="G24" s="125"/>
+      <c r="H24" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="243">
+        <v>21</v>
+      </c>
+      <c r="J24" s="87" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="125"/>
+      <c r="L24" s="125"/>
+      <c r="M24" s="125"/>
+      <c r="N24" s="125"/>
+      <c r="O24" s="125"/>
+      <c r="P24" s="239" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q24" s="244">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="244">
+        <v>22</v>
+      </c>
+      <c r="B25" s="209" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="243">
+        <v>22</v>
+      </c>
+      <c r="J25" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="240" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q25" s="244">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="167" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="168"/>
+      <c r="E26" s="168"/>
+      <c r="F26" s="168"/>
+      <c r="G26" s="169"/>
+      <c r="K26" s="167" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="168"/>
+      <c r="M26" s="168"/>
+      <c r="N26" s="168"/>
+      <c r="O26" s="169"/>
+    </row>
+    <row r="27" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="170"/>
+      <c r="D27" s="171"/>
+      <c r="E27" s="171"/>
+      <c r="F27" s="171"/>
+      <c r="G27" s="172"/>
+      <c r="K27" s="170"/>
+      <c r="L27" s="171"/>
+      <c r="M27" s="171"/>
+      <c r="N27" s="171"/>
+      <c r="O27" s="172"/>
+    </row>
+    <row r="28" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="241">
+        <v>1</v>
+      </c>
+      <c r="C28" s="241">
+        <v>2</v>
+      </c>
+      <c r="D28" s="241">
+        <v>3</v>
+      </c>
+      <c r="E28" s="241">
+        <v>4</v>
+      </c>
+      <c r="F28" s="241">
+        <v>5</v>
+      </c>
+      <c r="G28" s="242">
+        <v>6</v>
+      </c>
+      <c r="H28" s="242">
+        <v>7</v>
+      </c>
+      <c r="I28" s="242"/>
+      <c r="J28" s="241">
+        <v>7</v>
+      </c>
+      <c r="K28" s="241">
+        <v>6</v>
+      </c>
+      <c r="L28" s="241">
+        <v>5</v>
+      </c>
+      <c r="M28" s="241">
+        <v>4</v>
+      </c>
+      <c r="N28" s="241">
+        <v>3</v>
+      </c>
+      <c r="O28" s="241">
+        <v>2</v>
+      </c>
+      <c r="P28" s="241">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="15"/>
+    </row>
+    <row r="29" spans="1:17" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:17" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:17" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:17" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="41.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="K19:O24"/>
+    <mergeCell ref="K26:O27"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="N10:O11"/>
+    <mergeCell ref="N13:O14"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="C19:G24"/>
+    <mergeCell ref="C26:G27"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="88" fitToWidth="2" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;8&amp;D&amp;R&amp;8&amp;Z&amp;F</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>